<commit_message>
[5] Darstellung der Sprints in Tabelle.
</commit_message>
<xml_diff>
--- a/ProductBacklog/Sprints.xlsx
+++ b/ProductBacklog/Sprints.xlsx
@@ -31,16 +31,16 @@
     <t>EndDate</t>
   </si>
   <si>
-    <t>ActualCapacity</t>
-  </si>
-  <si>
     <t>EffortDone</t>
   </si>
   <si>
-    <t>PlannedCapacity</t>
-  </si>
-  <si>
-    <t>PlannedEffort</t>
+    <t>CapacityForecast</t>
+  </si>
+  <si>
+    <t>EffortForecast</t>
+  </si>
+  <si>
+    <t>CapacityDone</t>
   </si>
 </sst>
 </file>
@@ -383,7 +383,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -408,16 +408,16 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
[10] Effort-Forecast für Durchschnittliche Geschwindigkeit anzeigen.
</commit_message>
<xml_diff>
--- a/ProductBacklog/Sprints.xlsx
+++ b/ProductBacklog/Sprints.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sprints" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Sprint 1</t>
   </si>
@@ -41,6 +41,12 @@
   </si>
   <si>
     <t>CapacityDone</t>
+  </si>
+  <si>
+    <t>Forecast</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -380,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="I4" sqref="I4:L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -397,7 +403,7 @@
     <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -419,8 +425,14 @@
       <c r="G1" t="s">
         <v>5</v>
       </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -442,8 +454,24 @@
       <c r="G2">
         <v>0.5</v>
       </c>
+      <c r="I2">
+        <f>IF(D2&lt;&gt;"",E2/D2,"")</f>
+        <v>1</v>
+      </c>
+      <c r="J2">
+        <f>I2*D2</f>
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <f>IF(F2&lt;&gt;"",G2/F2,"")</f>
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="L2">
+        <f>K2*F2</f>
+        <v>0.5</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -458,6 +486,28 @@
       </c>
       <c r="E3">
         <v>6.5</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>7.5</v>
+      </c>
+      <c r="I3">
+        <f>IF(D3&lt;&gt;"",E3/D3,"")</f>
+        <v>0.8125</v>
+      </c>
+      <c r="J3">
+        <f>I3*D3</f>
+        <v>6.5</v>
+      </c>
+      <c r="K3">
+        <f>IF(F3&lt;&gt;"",G3/F3,"")</f>
+        <v>0.75</v>
+      </c>
+      <c r="L3">
+        <f>K3*F3</f>
+        <v>7.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>